<commit_message>
Separate log file for each person in immediateRun
- added customize sendLog to each function
- changed the Auth class so it will fit to our new sendLog completeFromAka
- added new singelton class for redis
</commit_message>
<xml_diff>
--- a/src/config/dataSourcesMap.xlsx
+++ b/src/config/dataSourcesMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chaga\Desktop\teem UI\karting\src\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2058A4E1-5813-4AFD-8EB3-AD4F96FF0742}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F948BDF-9E9C-49E8-98A1-C2FA75117080}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>es1</t>
   </si>
@@ -69,14 +69,29 @@
     <t>ads6</t>
   </si>
   <si>
-    <t>Music</t>
+    <t>city1</t>
+  </si>
+  <si>
+    <t>city2</t>
+  </si>
+  <si>
+    <t>city3</t>
+  </si>
+  <si>
+    <t>city4</t>
+  </si>
+  <si>
+    <t>city5</t>
+  </si>
+  <si>
+    <t>city6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -86,6 +101,10 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -330,7 +349,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -363,6 +382,9 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -371,6 +393,9 @@
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -379,6 +404,9 @@
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -387,6 +415,9 @@
       <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -394,6 +425,9 @@
       </c>
       <c r="D6" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1391,6 +1425,7 @@
     <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>

</xml_diff>

<commit_message>
fixed last pull request, adding mm
</commit_message>
<xml_diff>
--- a/src/config/dataSourcesMap.xlsx
+++ b/src/config/dataSourcesMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chaga\Desktop\teem UI\karting\src\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rani Jammal\karting\src\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F948BDF-9E9C-49E8-98A1-C2FA75117080}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7B8F96-46DF-451B-99BC-0A4602C98AB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6705" yWindow="975" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataSources" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>es1</t>
   </si>
@@ -85,6 +85,24 @@
   </si>
   <si>
     <t>city6</t>
+  </si>
+  <si>
+    <t>mm1</t>
+  </si>
+  <si>
+    <t>mm2</t>
+  </si>
+  <si>
+    <t>mm3</t>
+  </si>
+  <si>
+    <t>mm4</t>
+  </si>
+  <si>
+    <t>mm5</t>
+  </si>
+  <si>
+    <t>mm6</t>
   </si>
 </sst>
 </file>
@@ -346,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -358,7 +376,7 @@
     <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -371,8 +389,11 @@
       <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -385,8 +406,11 @@
       <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -396,8 +420,11 @@
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -407,8 +434,11 @@
       <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -418,8 +448,11 @@
       <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -429,17 +462,20 @@
       <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>